<commit_message>
finished template input file, added some code
</commit_message>
<xml_diff>
--- a/template_input.xlsx
+++ b/template_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chujiahe/Desktop/propens-pandapower/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26EF4E9-81AC-D74B-8602-9D7D1EA374CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4442EDDA-BF5F-9649-A7EB-494109F449B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="2100" windowWidth="25160" windowHeight="15820" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -19,20 +19,25 @@
     <sheet name="switch" sheetId="11" r:id="rId4"/>
     <sheet name="load" sheetId="3" r:id="rId5"/>
     <sheet name="motor" sheetId="13" r:id="rId6"/>
-    <sheet name="ext_grid" sheetId="4" r:id="rId7"/>
-    <sheet name="generator" sheetId="12" r:id="rId8"/>
-    <sheet name="trafo" sheetId="6" r:id="rId9"/>
-    <sheet name="line_std_types" sheetId="7" r:id="rId10"/>
-    <sheet name="trafo_std_types" sheetId="8" r:id="rId11"/>
-    <sheet name="trafo3w_std_types" sheetId="9" r:id="rId12"/>
-    <sheet name="dtypes" sheetId="10" r:id="rId13"/>
+    <sheet name="asymmetric_load" sheetId="14" r:id="rId7"/>
+    <sheet name="static_gen" sheetId="15" r:id="rId8"/>
+    <sheet name="ext_grid" sheetId="4" r:id="rId9"/>
+    <sheet name="trafo" sheetId="6" r:id="rId10"/>
+    <sheet name="generator" sheetId="12" r:id="rId11"/>
+    <sheet name="impedance" sheetId="16" r:id="rId12"/>
+    <sheet name="dc_line" sheetId="17" r:id="rId13"/>
+    <sheet name="storage" sheetId="18" r:id="rId14"/>
+    <sheet name="line_std_types" sheetId="7" r:id="rId15"/>
+    <sheet name="trafo_std_types" sheetId="8" r:id="rId16"/>
+    <sheet name="trafo3w_std_types" sheetId="9" r:id="rId17"/>
+    <sheet name="dtypes" sheetId="10" r:id="rId18"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="215">
   <si>
     <t>version</t>
   </si>
@@ -608,13 +613,82 @@
   </si>
   <si>
     <t>rx</t>
+  </si>
+  <si>
+    <t>p_a_mw</t>
+  </si>
+  <si>
+    <t>q_a_mvar</t>
+  </si>
+  <si>
+    <t>p_b_mw</t>
+  </si>
+  <si>
+    <t>q_b_mvar</t>
+  </si>
+  <si>
+    <t>p_c_mw</t>
+  </si>
+  <si>
+    <t>q_c_mvar</t>
+  </si>
+  <si>
+    <t>current_source</t>
+  </si>
+  <si>
+    <t>rft_pu</t>
+  </si>
+  <si>
+    <t>xft_pu</t>
+  </si>
+  <si>
+    <t>rtf_pu</t>
+  </si>
+  <si>
+    <t>xtf_pu</t>
+  </si>
+  <si>
+    <t>loss_percent</t>
+  </si>
+  <si>
+    <t>loss_mw</t>
+  </si>
+  <si>
+    <t>vm_from_pu</t>
+  </si>
+  <si>
+    <t>vm_to_pu</t>
+  </si>
+  <si>
+    <t>max_p_mw</t>
+  </si>
+  <si>
+    <t>min_q_from_mvar</t>
+  </si>
+  <si>
+    <t>min_q_to_mvar</t>
+  </si>
+  <si>
+    <t>max_q_from_mvar</t>
+  </si>
+  <si>
+    <t>max_q_to_mvar</t>
+  </si>
+  <si>
+    <t>soc_percent</t>
+  </si>
+  <si>
+    <t>min_e_mwh</t>
+  </si>
+  <si>
+    <t>max_e_mwh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -636,6 +710,22 @@
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -673,13 +763,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1020,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1066,6 +1158,384 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:X2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0.16</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>0.4</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>1.2</v>
+      </c>
+      <c r="K2">
+        <v>0.38</v>
+      </c>
+      <c r="L2">
+        <v>0.26</v>
+      </c>
+      <c r="M2">
+        <v>150</v>
+      </c>
+      <c r="U2" t="b">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{284F317A-3D29-9745-938E-3F12A757720B}">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{215CEB82-8379-0044-A4DE-65391D83CD57}">
+  <dimension ref="B1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5222D357-E374-C940-A594-350F6CF2C6F8}">
+  <dimension ref="B1:P1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D9302E-8D96-E04C-A032-2E671798540C}">
+  <dimension ref="B1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H57"/>
   <sheetViews>
@@ -2542,7 +3012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
@@ -3411,7 +3881,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:W3"/>
   <sheetViews>
@@ -3634,7 +4104,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D58"/>
   <sheetViews>
@@ -5496,10 +5966,117 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047FF36C-78BB-0949-AD1E-78FDFDB70111}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49101B8C-97BD-E04E-B065-4BAAF445EB39}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
@@ -5542,227 +6119,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{284F317A-3D29-9745-938E-3F12A757720B}">
-  <dimension ref="A1:M11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="3"/>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:X2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>0.16</v>
-      </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-      <c r="H2">
-        <v>0.4</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
-      </c>
-      <c r="J2">
-        <v>1.2</v>
-      </c>
-      <c r="K2">
-        <v>0.38</v>
-      </c>
-      <c r="L2">
-        <v>0.26</v>
-      </c>
-      <c r="M2">
-        <v>150</v>
-      </c>
-      <c r="U2" t="b">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>1</v>
-      </c>
-      <c r="W2">
-        <v>1</v>
-      </c>
-      <c r="X2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
finished read_input function, adjusted input file template
</commit_message>
<xml_diff>
--- a/template_input.xlsx
+++ b/template_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chujiahe/Desktop/propens-pandapower/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4442EDDA-BF5F-9649-A7EB-494109F449B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA85AEF-9C46-6F45-A574-485BE7EE9850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -20,24 +20,37 @@
     <sheet name="load" sheetId="3" r:id="rId5"/>
     <sheet name="motor" sheetId="13" r:id="rId6"/>
     <sheet name="asymmetric_load" sheetId="14" r:id="rId7"/>
-    <sheet name="static_gen" sheetId="15" r:id="rId8"/>
+    <sheet name="sgen" sheetId="15" r:id="rId8"/>
     <sheet name="ext_grid" sheetId="4" r:id="rId9"/>
-    <sheet name="trafo" sheetId="6" r:id="rId10"/>
-    <sheet name="generator" sheetId="12" r:id="rId11"/>
+    <sheet name="transformer" sheetId="6" r:id="rId10"/>
+    <sheet name="gen" sheetId="12" r:id="rId11"/>
     <sheet name="impedance" sheetId="16" r:id="rId12"/>
-    <sheet name="dc_line" sheetId="17" r:id="rId13"/>
+    <sheet name="dcline" sheetId="17" r:id="rId13"/>
     <sheet name="storage" sheetId="18" r:id="rId14"/>
     <sheet name="line_std_types" sheetId="7" r:id="rId15"/>
     <sheet name="trafo_std_types" sheetId="8" r:id="rId16"/>
     <sheet name="trafo3w_std_types" sheetId="9" r:id="rId17"/>
     <sheet name="dtypes" sheetId="10" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="206">
   <si>
     <t>version</t>
   </si>
@@ -141,39 +154,6 @@
     <t>line_1_2</t>
   </si>
   <si>
-    <t>line_1_3</t>
-  </si>
-  <si>
-    <t>line_1_4</t>
-  </si>
-  <si>
-    <t>line_1_5</t>
-  </si>
-  <si>
-    <t>line_1_6</t>
-  </si>
-  <si>
-    <t>line_1_7</t>
-  </si>
-  <si>
-    <t>line_1_8</t>
-  </si>
-  <si>
-    <t>line_1_9</t>
-  </si>
-  <si>
-    <t>line_1_10</t>
-  </si>
-  <si>
-    <t>line_1_11</t>
-  </si>
-  <si>
-    <t>line_1_12</t>
-  </si>
-  <si>
-    <t>line_1_13</t>
-  </si>
-  <si>
     <t>NFA2X 4x70</t>
   </si>
   <si>
@@ -582,9 +562,6 @@
     <t>in_ka</t>
   </si>
   <si>
-    <t>l</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -682,13 +659,22 @@
   </si>
   <si>
     <t>max_e_mwh</t>
+  </si>
+  <si>
+    <t>r0_ohm_per_km</t>
+  </si>
+  <si>
+    <t>x0_ohm_per_km</t>
+  </si>
+  <si>
+    <t>c0_nf_per_km</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -727,6 +713,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF404040"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF404040"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -763,7 +762,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -772,6 +771,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1112,7 +1125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
@@ -1161,70 +1174,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1:U1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="20.1640625" style="12" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>31</v>
@@ -1241,10 +1259,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" t="s">
-        <v>65</v>
+        <v>53</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1299,7 +1317,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1322,31 +1340,29 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>0</v>
-      </c>
+      <c r="A2" s="3"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -1401,16 +1417,16 @@
         <v>23</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>4</v>
@@ -1429,7 +1445,7 @@
   <dimension ref="B1:P1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1448,31 +1464,31 @@
         <v>14</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>9</v>
@@ -1511,13 +1527,13 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>18</v>
@@ -1560,15 +1576,15 @@
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B2">
         <v>210</v>
@@ -1583,7 +1599,7 @@
         <v>0.14199999999999999</v>
       </c>
       <c r="F2" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G2">
         <v>50</v>
@@ -1594,7 +1610,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B3">
         <v>264</v>
@@ -1609,7 +1625,7 @@
         <v>0.24199999999999999</v>
       </c>
       <c r="F3" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G3">
         <v>120</v>
@@ -1620,7 +1636,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B4">
         <v>261</v>
@@ -1635,7 +1651,7 @@
         <v>0.27</v>
       </c>
       <c r="F4" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G4">
         <v>150</v>
@@ -1646,7 +1662,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <v>216</v>
@@ -1661,7 +1677,7 @@
         <v>0.252</v>
       </c>
       <c r="F5" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G5">
         <v>95</v>
@@ -1672,7 +1688,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B6">
         <v>273</v>
@@ -1687,7 +1703,7 @@
         <v>0.36199999999999999</v>
       </c>
       <c r="F6" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G6">
         <v>185</v>
@@ -1698,7 +1714,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B7">
         <v>304</v>
@@ -1713,7 +1729,7 @@
         <v>0.42099999999999999</v>
       </c>
       <c r="F7" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G7">
         <v>240</v>
@@ -1724,7 +1740,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B8">
         <v>315</v>
@@ -1739,7 +1755,7 @@
         <v>0.249</v>
       </c>
       <c r="F8" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G8">
         <v>95</v>
@@ -1750,7 +1766,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B9">
         <v>406</v>
@@ -1765,7 +1781,7 @@
         <v>0.35799999999999998</v>
       </c>
       <c r="F9" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G9">
         <v>185</v>
@@ -1776,7 +1792,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B10">
         <v>456</v>
@@ -1791,7 +1807,7 @@
         <v>0.41599999999999998</v>
       </c>
       <c r="F10" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G10">
         <v>240</v>
@@ -1802,7 +1818,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B11">
         <v>250</v>
@@ -1817,7 +1833,7 @@
         <v>0.31900000000000001</v>
       </c>
       <c r="F11" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G11">
         <v>150</v>
@@ -1828,7 +1844,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B12">
         <v>230</v>
@@ -1843,7 +1859,7 @@
         <v>0.28299999999999997</v>
       </c>
       <c r="F12" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G12">
         <v>120</v>
@@ -1854,7 +1870,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B13">
         <v>190</v>
@@ -1869,7 +1885,7 @@
         <v>0.22</v>
       </c>
       <c r="F13" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G13">
         <v>70</v>
@@ -1880,7 +1896,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B14">
         <v>360</v>
@@ -1895,7 +1911,7 @@
         <v>0.315</v>
       </c>
       <c r="F14" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G14">
         <v>150</v>
@@ -1906,7 +1922,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B15">
         <v>340</v>
@@ -1921,7 +1937,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="F15" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G15">
         <v>120</v>
@@ -1932,7 +1948,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B16">
         <v>280</v>
@@ -1947,7 +1963,7 @@
         <v>0.217</v>
       </c>
       <c r="F16" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G16">
         <v>70</v>
@@ -1958,7 +1974,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B17">
         <v>112</v>
@@ -1973,7 +1989,7 @@
         <v>0.36599999999999999</v>
       </c>
       <c r="F17" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G17">
         <v>120</v>
@@ -1984,7 +2000,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B18">
         <v>125</v>
@@ -1999,7 +2015,7 @@
         <v>0.45700000000000002</v>
       </c>
       <c r="F18" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G18">
         <v>185</v>
@@ -2010,7 +2026,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B19">
         <v>135</v>
@@ -2025,7 +2041,7 @@
         <v>0.52600000000000002</v>
       </c>
       <c r="F19" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G19">
         <v>240</v>
@@ -2036,7 +2052,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B20">
         <v>144</v>
@@ -2051,7 +2067,7 @@
         <v>0.58799999999999997</v>
       </c>
       <c r="F20" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G20">
         <v>300</v>
@@ -2062,7 +2078,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B21">
         <v>11</v>
@@ -2077,7 +2093,7 @@
         <v>0.105</v>
       </c>
       <c r="F21" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G21">
         <v>16</v>
@@ -2088,7 +2104,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B22">
         <v>11.25</v>
@@ -2103,7 +2119,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="F22" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G22">
         <v>24</v>
@@ -2114,7 +2130,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B23">
         <v>12.2</v>
@@ -2129,7 +2145,7 @@
         <v>0.21</v>
       </c>
       <c r="F23" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G23">
         <v>48</v>
@@ -2140,7 +2156,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B24">
         <v>13.2</v>
@@ -2155,7 +2171,7 @@
         <v>0.35</v>
       </c>
       <c r="F24" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G24">
         <v>94</v>
@@ -2166,7 +2182,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B25">
         <v>9.6999999999999993</v>
@@ -2181,7 +2197,7 @@
         <v>0.17</v>
       </c>
       <c r="F25" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G25">
         <v>34</v>
@@ -2192,7 +2208,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B26">
         <v>10.1</v>
@@ -2207,7 +2223,7 @@
         <v>0.21</v>
       </c>
       <c r="F26" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G26">
         <v>48</v>
@@ -2218,7 +2234,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B27">
         <v>10.4</v>
@@ -2233,7 +2249,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="F27" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G27">
         <v>70</v>
@@ -2244,7 +2260,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B28">
         <v>10.75</v>
@@ -2259,7 +2275,7 @@
         <v>0.35</v>
       </c>
       <c r="F28" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G28">
         <v>94</v>
@@ -2270,7 +2286,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B29">
         <v>11.1</v>
@@ -2285,7 +2301,7 @@
         <v>0.41</v>
       </c>
       <c r="F29" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G29">
         <v>122</v>
@@ -2296,7 +2312,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B30">
         <v>11.25</v>
@@ -2311,7 +2327,7 @@
         <v>0.47</v>
       </c>
       <c r="F30" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G30">
         <v>149</v>
@@ -2322,7 +2338,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B31">
         <v>9.15</v>
@@ -2337,7 +2353,7 @@
         <v>0.17</v>
       </c>
       <c r="F31" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G31">
         <v>34</v>
@@ -2348,7 +2364,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B32">
         <v>9.5</v>
@@ -2363,7 +2379,7 @@
         <v>0.21</v>
       </c>
       <c r="F32" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G32">
         <v>48</v>
@@ -2374,7 +2390,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B33">
         <v>9.6999999999999993</v>
@@ -2389,7 +2405,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="F33" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G33">
         <v>70</v>
@@ -2400,7 +2416,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B34">
         <v>10</v>
@@ -2415,7 +2431,7 @@
         <v>0.35</v>
       </c>
       <c r="F34" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G34">
         <v>94</v>
@@ -2426,7 +2442,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B35">
         <v>10.3</v>
@@ -2441,7 +2457,7 @@
         <v>0.41</v>
       </c>
       <c r="F35" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G35">
         <v>122</v>
@@ -2452,7 +2468,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B36">
         <v>10.5</v>
@@ -2467,7 +2483,7 @@
         <v>0.47</v>
       </c>
       <c r="F36" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G36">
         <v>149</v>
@@ -2478,7 +2494,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B37">
         <v>10.75</v>
@@ -2493,7 +2509,7 @@
         <v>0.53500000000000003</v>
       </c>
       <c r="F37" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G37">
         <v>184</v>
@@ -2504,7 +2520,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B38">
         <v>11</v>
@@ -2519,7 +2535,7 @@
         <v>0.64500000000000002</v>
       </c>
       <c r="F38" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G38">
         <v>243</v>
@@ -2530,7 +2546,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B39">
         <v>8</v>
@@ -2545,7 +2561,7 @@
         <v>0.21</v>
       </c>
       <c r="F39" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G39">
         <v>48</v>
@@ -2556,7 +2572,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B40">
         <v>8.4</v>
@@ -2571,7 +2587,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="F40" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G40">
         <v>70</v>
@@ -2582,7 +2598,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B41">
         <v>8.65</v>
@@ -2597,7 +2613,7 @@
         <v>0.35</v>
       </c>
       <c r="F41" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G41">
         <v>94</v>
@@ -2608,7 +2624,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B42">
         <v>8.5</v>
@@ -2623,7 +2639,7 @@
         <v>0.41</v>
       </c>
       <c r="F42" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G42">
         <v>122</v>
@@ -2634,7 +2650,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B43">
         <v>8.75</v>
@@ -2649,7 +2665,7 @@
         <v>0.47</v>
       </c>
       <c r="F43" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G43">
         <v>149</v>
@@ -2660,7 +2676,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B44">
         <v>8.8000000000000007</v>
@@ -2675,7 +2691,7 @@
         <v>0.53500000000000003</v>
       </c>
       <c r="F44" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G44">
         <v>184</v>
@@ -2686,7 +2702,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B45">
         <v>9</v>
@@ -2701,7 +2717,7 @@
         <v>0.64500000000000002</v>
       </c>
       <c r="F45" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G45">
         <v>243</v>
@@ -2712,7 +2728,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B46">
         <v>9.1999999999999993</v>
@@ -2727,7 +2743,7 @@
         <v>0.74</v>
       </c>
       <c r="F46" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G46">
         <v>305</v>
@@ -2738,7 +2754,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B47">
         <v>9.75</v>
@@ -2753,7 +2769,7 @@
         <v>0.96</v>
       </c>
       <c r="F47" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G47">
         <v>490</v>
@@ -2764,7 +2780,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B48">
         <v>9.9499999999999993</v>
@@ -2779,7 +2795,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="F48" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G48">
         <v>679</v>
@@ -2790,7 +2806,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B49">
         <v>10</v>
@@ -2805,7 +2821,7 @@
         <v>0.96</v>
       </c>
       <c r="F49" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G49">
         <v>490</v>
@@ -2816,7 +2832,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B50">
         <v>11.7</v>
@@ -2831,7 +2847,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="F50" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G50">
         <v>679</v>
@@ -2842,7 +2858,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B51">
         <v>11</v>
@@ -2857,7 +2873,7 @@
         <v>0.96</v>
       </c>
       <c r="F51" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G51">
         <v>490</v>
@@ -2868,7 +2884,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B52">
         <v>14.6</v>
@@ -2883,7 +2899,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="F52" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G52">
         <v>679</v>
@@ -2894,7 +2910,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -2909,7 +2925,7 @@
         <v>0.27</v>
       </c>
       <c r="F53" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G53">
         <v>70</v>
@@ -2917,7 +2933,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B54">
         <v>670</v>
@@ -2932,7 +2948,7 @@
         <v>0.14099999999999999</v>
       </c>
       <c r="F54" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G54">
         <v>50</v>
@@ -2940,7 +2956,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B55">
         <v>830</v>
@@ -2955,7 +2971,7 @@
         <v>0.27500000000000002</v>
       </c>
       <c r="F55" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G55">
         <v>150</v>
@@ -2963,7 +2979,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B56">
         <v>830</v>
@@ -2978,7 +2994,7 @@
         <v>0.313</v>
       </c>
       <c r="F56" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G56">
         <v>185</v>
@@ -2986,7 +3002,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -3001,7 +3017,7 @@
         <v>0.156</v>
       </c>
       <c r="F57" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G57">
         <v>35</v>
@@ -3022,57 +3038,57 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B2">
         <v>0.06</v>
@@ -3099,10 +3115,10 @@
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="K2" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -3125,7 +3141,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B3">
         <v>0.06</v>
@@ -3152,10 +3168,10 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="K3" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -3178,7 +3194,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B4">
         <v>0.04</v>
@@ -3205,10 +3221,10 @@
         <v>150</v>
       </c>
       <c r="J4" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="K4" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -3231,7 +3247,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B5">
         <v>0.05</v>
@@ -3258,10 +3274,10 @@
         <v>150</v>
       </c>
       <c r="J5" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="K5" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -3284,7 +3300,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B6">
         <v>7.0000000000000007E-2</v>
@@ -3311,10 +3327,10 @@
         <v>150</v>
       </c>
       <c r="J6" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="K6" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -3337,7 +3353,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="B7">
         <v>0.04</v>
@@ -3364,10 +3380,10 @@
         <v>150</v>
       </c>
       <c r="J7" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="K7" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -3390,7 +3406,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B8">
         <v>0.05</v>
@@ -3417,10 +3433,10 @@
         <v>150</v>
       </c>
       <c r="J8" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="K8" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -3443,7 +3459,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B9">
         <v>7.0000000000000007E-2</v>
@@ -3470,10 +3486,10 @@
         <v>150</v>
       </c>
       <c r="J9" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="K9" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -3496,7 +3512,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B10">
         <v>0.32</v>
@@ -3523,10 +3539,10 @@
         <v>150</v>
       </c>
       <c r="J10" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="K10" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -3549,7 +3565,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B11">
         <v>0.33750000000000002</v>
@@ -3576,10 +3592,10 @@
         <v>150</v>
       </c>
       <c r="J11" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="K11" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -3602,7 +3618,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B12">
         <v>0.26190000000000002</v>
@@ -3629,10 +3645,10 @@
         <v>150</v>
       </c>
       <c r="J12" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="K12" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -3655,7 +3671,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B13">
         <v>0.24</v>
@@ -3682,10 +3698,10 @@
         <v>150</v>
       </c>
       <c r="J13" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="K13" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -3708,7 +3724,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B14">
         <v>0.23749999999999999</v>
@@ -3735,10 +3751,10 @@
         <v>150</v>
       </c>
       <c r="J14" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="K14" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -3761,7 +3777,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="B15">
         <v>0.18729999999999999</v>
@@ -3788,10 +3804,10 @@
         <v>150</v>
       </c>
       <c r="J15" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="K15" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -3814,7 +3830,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B16">
         <v>0.25</v>
@@ -3841,12 +3857,12 @@
         <v>150</v>
       </c>
       <c r="J16" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B17">
         <v>0.26</v>
@@ -3873,7 +3889,7 @@
         <v>150</v>
       </c>
       <c r="J17" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -3891,75 +3907,75 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B2">
         <v>63</v>
@@ -4010,10 +4026,10 @@
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="S2" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="T2">
         <v>0</v>
@@ -4030,7 +4046,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="B3">
         <v>63</v>
@@ -4081,10 +4097,10 @@
         <v>0</v>
       </c>
       <c r="R3" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="S3" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -4116,13 +4132,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4136,7 +4152,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4150,7 +4166,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4164,7 +4180,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4178,7 +4194,7 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4192,7 +4208,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4200,13 +4216,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4214,13 +4230,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4228,13 +4244,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4242,13 +4258,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -4256,13 +4272,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4270,13 +4286,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -4284,13 +4300,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4298,13 +4314,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -4312,13 +4328,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -4326,13 +4342,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -4340,13 +4356,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -4354,13 +4370,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C18" t="s">
         <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -4368,13 +4384,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C19" t="s">
         <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -4382,13 +4398,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C20" t="s">
         <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -4396,13 +4412,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -4410,13 +4426,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -4424,13 +4440,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C23" t="s">
         <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -4438,13 +4454,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C24" t="s">
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -4452,13 +4468,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C25" t="s">
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -4466,13 +4482,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C26" t="s">
         <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -4480,13 +4496,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C27" t="s">
         <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -4494,13 +4510,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C28" t="s">
         <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -4508,13 +4524,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C29" t="s">
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -4522,13 +4538,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C30" t="s">
         <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -4536,13 +4552,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C31" t="s">
         <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -4550,13 +4566,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C32" t="s">
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -4564,13 +4580,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C33" t="s">
         <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -4578,13 +4594,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -4592,13 +4608,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C35" t="s">
         <v>9</v>
       </c>
       <c r="D35" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -4606,13 +4622,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -4620,13 +4636,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C37" t="s">
         <v>21</v>
       </c>
       <c r="D37" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -4634,13 +4650,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C38" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D38" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -4648,13 +4664,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C39" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -4662,13 +4678,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -4676,13 +4692,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C41" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D41" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -4690,13 +4706,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C42" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="D42" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -4704,13 +4720,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C43" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D43" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -4718,13 +4734,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C44" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D44" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -4732,13 +4748,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C45" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="D45" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -4746,13 +4762,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C46" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D46" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -4760,13 +4776,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C47" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D47" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -4774,13 +4790,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C48" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D48" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -4788,13 +4804,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C49" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D49" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -4802,13 +4818,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C50" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="D50" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -4816,13 +4832,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C51" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D51" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -4830,13 +4846,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C52" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="D52" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -4844,13 +4860,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C53" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D53" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -4858,13 +4874,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C54" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D54" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -4872,13 +4888,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C55" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="D55" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -4886,13 +4902,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C56" t="s">
         <v>31</v>
       </c>
       <c r="D56" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -4900,13 +4916,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C57" t="s">
         <v>30</v>
       </c>
       <c r="D57" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -4914,13 +4930,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C58" t="s">
         <v>9</v>
       </c>
       <c r="D58" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -4933,7 +4949,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4994,7 +5010,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="C4">
         <v>0.4</v>
@@ -5011,7 +5027,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="C5">
         <v>0.4</v>
@@ -5030,28 +5046,37 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="8.83203125" style="12"/>
+    <col min="6" max="6" width="8.83203125" style="15"/>
+    <col min="7" max="7" width="21.5" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" customWidth="1"/>
+    <col min="9" max="9" width="25.83203125" customWidth="1"/>
+    <col min="10" max="13" width="22.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A1" s="6"/>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="13" t="s">
         <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -5066,632 +5091,200 @@
       <c r="J1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="14">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="14">
         <v>2</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="14">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="6">
         <v>0.443</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="6">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
+      <c r="I2" s="6">
+        <v>0</v>
+      </c>
+      <c r="J2" s="6">
+        <v>0</v>
+      </c>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6">
         <v>0.27</v>
       </c>
-      <c r="L2">
+      <c r="O2" s="6">
         <v>1</v>
       </c>
-      <c r="M2">
+      <c r="P2" s="6">
         <v>1</v>
       </c>
-      <c r="N2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O2" t="b">
+      <c r="Q2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="14">
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="14">
         <v>3</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="14">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="6">
         <v>0.443</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="6">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6">
         <v>0.27</v>
       </c>
-      <c r="L3">
+      <c r="O3" s="6">
         <v>1</v>
       </c>
-      <c r="M3">
+      <c r="P3" s="6">
         <v>1</v>
       </c>
-      <c r="N3" t="s">
-        <v>46</v>
-      </c>
-      <c r="O3" t="b">
+      <c r="Q3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="G4">
-        <v>0.443</v>
-      </c>
-      <c r="H4">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0.27</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4" t="s">
-        <v>46</v>
-      </c>
-      <c r="O4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="G5">
-        <v>0.443</v>
-      </c>
-      <c r="H5">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0.27</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5" t="s">
-        <v>46</v>
-      </c>
-      <c r="O5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6">
-        <v>6</v>
-      </c>
-      <c r="F6">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="G6">
-        <v>0.443</v>
-      </c>
-      <c r="H6">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0.27</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6" t="s">
-        <v>46</v>
-      </c>
-      <c r="O6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-      <c r="E7">
-        <v>7</v>
-      </c>
-      <c r="F7">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="G7">
-        <v>0.443</v>
-      </c>
-      <c r="H7">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0.27</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7" t="s">
-        <v>46</v>
-      </c>
-      <c r="O7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8">
-        <v>7</v>
-      </c>
-      <c r="E8">
-        <v>8</v>
-      </c>
-      <c r="F8">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="G8">
-        <v>0.443</v>
-      </c>
-      <c r="H8">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0.27</v>
-      </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8" t="s">
-        <v>46</v>
-      </c>
-      <c r="O8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9">
-        <v>8</v>
-      </c>
-      <c r="E9">
-        <v>9</v>
-      </c>
-      <c r="F9">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="G9">
-        <v>0.443</v>
-      </c>
-      <c r="H9">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0.27</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9" t="s">
-        <v>46</v>
-      </c>
-      <c r="O9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10">
-        <v>9</v>
-      </c>
-      <c r="E10">
-        <v>10</v>
-      </c>
-      <c r="F10">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="G10">
-        <v>0.443</v>
-      </c>
-      <c r="H10">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0.27</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="N10" t="s">
-        <v>46</v>
-      </c>
-      <c r="O10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11">
-        <v>10</v>
-      </c>
-      <c r="E11">
-        <v>11</v>
-      </c>
-      <c r="F11">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="G11">
-        <v>0.443</v>
-      </c>
-      <c r="H11">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0.27</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11" t="s">
-        <v>46</v>
-      </c>
-      <c r="O11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12">
-        <v>11</v>
-      </c>
-      <c r="E12">
-        <v>12</v>
-      </c>
-      <c r="F12">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="G12">
-        <v>0.443</v>
-      </c>
-      <c r="H12">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0.27</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="N12" t="s">
-        <v>46</v>
-      </c>
-      <c r="O12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13">
-        <v>12</v>
-      </c>
-      <c r="E13">
-        <v>13</v>
-      </c>
-      <c r="F13">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="G13">
-        <v>0.443</v>
-      </c>
-      <c r="H13">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0.27</v>
-      </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13" t="s">
-        <v>46</v>
-      </c>
-      <c r="O13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14">
-        <v>13</v>
-      </c>
-      <c r="E14">
-        <v>14</v>
-      </c>
-      <c r="F14">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="G14">
-        <v>0.443</v>
-      </c>
-      <c r="H14">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0.27</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
-      <c r="N14" t="s">
-        <v>46</v>
-      </c>
-      <c r="O14" t="b">
-        <v>1</v>
-      </c>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5703,7 +5296,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5714,25 +5307,25 @@
         <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -5746,22 +5339,22 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>181</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -5909,7 +5502,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5922,25 +5515,25 @@
         <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>6</v>
@@ -5952,13 +5545,11 @@
         <v>9</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>0</v>
-      </c>
+      <c r="A2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5967,15 +5558,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047FF36C-78BB-0949-AD1E-78FDFDB70111}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="B1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
@@ -5983,22 +5574,22 @@
         <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>4</v>
@@ -6011,11 +5602,6 @@
       </c>
       <c r="M1" s="4" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6025,15 +5611,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49101B8C-97BD-E04E-B065-4BAAF445EB39}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="B1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
@@ -6059,12 +5645,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added geodata to bus parameters
</commit_message>
<xml_diff>
--- a/template_input.xlsx
+++ b/template_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chujiahe/Desktop/propens-pandapower/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA85AEF-9C46-6F45-A574-485BE7EE9850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142F4DFE-D147-8A4C-8E0C-8F88BE435127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="17600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="211">
   <si>
     <t>version</t>
   </si>
@@ -668,6 +668,21 @@
   </si>
   <si>
     <t>c0_nf_per_km</t>
+  </si>
+  <si>
+    <t>geodata</t>
+  </si>
+  <si>
+    <t>0, 0</t>
+  </si>
+  <si>
+    <t>0, 1</t>
+  </si>
+  <si>
+    <t>0, 2</t>
+  </si>
+  <si>
+    <t>0, 3</t>
   </si>
 </sst>
 </file>
@@ -762,7 +777,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -771,19 +786,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1174,20 +1186,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:U1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="20.1640625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1261,7 +1273,7 @@
       <c r="B2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>127</v>
       </c>
       <c r="D2">
@@ -1401,7 +1413,7 @@
   <dimension ref="B1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4946,15 +4958,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4967,11 +4979,14 @@
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4984,11 +4999,14 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="b">
+      <c r="F2" t="s">
+        <v>207</v>
+      </c>
+      <c r="G2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5001,11 +5019,14 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="b">
+      <c r="F3" t="s">
+        <v>208</v>
+      </c>
+      <c r="G3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -5018,11 +5039,14 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="b">
+      <c r="F4" t="s">
+        <v>209</v>
+      </c>
+      <c r="G4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -5035,7 +5059,10 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="b">
+      <c r="F5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G5" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5046,7 +5073,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
@@ -5054,29 +5081,28 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="8.83203125" style="12"/>
-    <col min="6" max="6" width="8.83203125" style="15"/>
+    <col min="3" max="3" width="8.83203125" style="10"/>
+    <col min="6" max="6" width="8.83203125" style="12"/>
     <col min="7" max="7" width="21.5" customWidth="1"/>
     <col min="8" max="8" width="17.83203125" customWidth="1"/>
     <col min="9" max="9" width="25.83203125" customWidth="1"/>
     <col min="10" max="13" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -5091,13 +5117,13 @@
       <c r="J1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>205</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -5115,176 +5141,104 @@
       <c r="R1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="12">
         <v>1</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="12">
         <v>2</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="12">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2">
         <v>0.443</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="I2" s="6">
-        <v>0</v>
-      </c>
-      <c r="J2" s="6">
-        <v>0</v>
-      </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6">
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="N2">
         <v>0.27</v>
       </c>
-      <c r="O2" s="6">
+      <c r="O2">
         <v>1</v>
       </c>
-      <c r="P2" s="6">
+      <c r="P2">
         <v>1</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" t="s">
         <v>35</v>
       </c>
-      <c r="R2" s="6" t="b">
+      <c r="R2" t="b">
         <v>1</v>
       </c>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="12">
         <v>2</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="12">
         <v>3</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="12">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3">
         <v>0.443</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="I3" s="6">
-        <v>0</v>
-      </c>
-      <c r="J3" s="6">
-        <v>0</v>
-      </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6">
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="N3">
         <v>0.27</v>
       </c>
-      <c r="O3" s="6">
+      <c r="O3">
         <v>1</v>
       </c>
-      <c r="P3" s="6">
+      <c r="P3">
         <v>1</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" t="s">
         <v>35</v>
       </c>
-      <c r="R3" s="6" t="b">
+      <c r="R3" t="b">
         <v>1</v>
       </c>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>